<commit_message>
updated producao again, and balde - base 03/02/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-02.xlsx
+++ b/first-atlas/producao_2026-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F51330-0131-40D6-A844-1D7869DC9047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31B710C-7181-4E50-A40F-F6EFCCC079D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,7 +2959,7 @@
         <v>187</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
updated producao and balde - base 06/02/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-02.xlsx
+++ b/first-atlas/producao_2026-02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29803"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAFCCA6-9218-42BB-ACEF-A565E36CA72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800C3843-C0B4-4279-8E53-08727C37B2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="742">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -1370,9 +1370,6 @@
     <t>AD FERREIRA TRANSPORTES LTDA</t>
   </si>
   <si>
-    <t>(A procuracao esta vencida) Procuracao com poderes de representacao junto a instituicoes financeiras podendo abrir e movimentar conta corrente com mandato vigente, assinada digitalmente pelo site do GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF.</t>
-  </si>
-  <si>
     <t>Documento de identificacao pois o apresentado estava ilegivel</t>
   </si>
   <si>
@@ -1872,6 +1869,402 @@
   </si>
   <si>
     <t xml:space="preserve"> Convencao de condominio atualizada e devidamente registrada em orgao competente.&lt;br&gt;&lt;br&gt;Convencao do condominio registrada no orgao competente</t>
+  </si>
+  <si>
+    <t>35448429000120</t>
+  </si>
+  <si>
+    <t>ANGELO P DE OLIVEIRA A P DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>Andrey de Souza Batista Bizao</t>
+  </si>
+  <si>
+    <t>BACKOFFICE</t>
+  </si>
+  <si>
+    <t>39579050000100</t>
+  </si>
+  <si>
+    <t>ALEQUES DALENOGARE FERRAZ</t>
+  </si>
+  <si>
+    <t>61243990000183</t>
+  </si>
+  <si>
+    <t>THIAGO BLANDY CAMPOS</t>
+  </si>
+  <si>
+    <t>61262125000184</t>
+  </si>
+  <si>
+    <t>ROUSE NEGOCIOS IMOBILIARIOS LTDA</t>
+  </si>
+  <si>
+    <t>14625988000199</t>
+  </si>
+  <si>
+    <t>NERMISON GONCALVES DA SILVA</t>
+  </si>
+  <si>
+    <t>37848814000190</t>
+  </si>
+  <si>
+    <t>ZEZINHO CONSTRUCOES LTDA</t>
+  </si>
+  <si>
+    <t>01580652000105</t>
+  </si>
+  <si>
+    <t>MCI INVESTIMENTOS E PARTICIPACOES LTDA</t>
+  </si>
+  <si>
+    <t>64934439000174</t>
+  </si>
+  <si>
+    <t>GUSTAVO DE CARVALHO RAGUZZANI CONSULTORIA</t>
+  </si>
+  <si>
+    <t>64493369000166</t>
+  </si>
+  <si>
+    <t>BEBIDARIA DA ORLA COMERCIO DE BEBIDAS E CONVENIENCIA LTDA</t>
+  </si>
+  <si>
+    <t>47306684000118</t>
+  </si>
+  <si>
+    <t>TJ COMERCIO DE MARMORES E GRANITOS LTDA</t>
+  </si>
+  <si>
+    <t>46659576000166</t>
+  </si>
+  <si>
+    <t>EVANDRO VINHAS MOVEIS LTDA</t>
+  </si>
+  <si>
+    <t>64936034000175</t>
+  </si>
+  <si>
+    <t>TEKTON SUPPLEMENTS LIMITADA</t>
+  </si>
+  <si>
+    <t>05747254000191</t>
+  </si>
+  <si>
+    <t>ACADJUR - ACADEMIA DE ESTUDOS JURIDICOS LTDA</t>
+  </si>
+  <si>
+    <t>03392931000170</t>
+  </si>
+  <si>
+    <t>DECK BAR 84 E CONVENIENCIA LTDA</t>
+  </si>
+  <si>
+    <t>64869693000136</t>
+  </si>
+  <si>
+    <t>FORT STEEL ARMACAO DE FERRAGENS LTDA</t>
+  </si>
+  <si>
+    <t>30043387000124</t>
+  </si>
+  <si>
+    <t>MBS FUTEBOL CLUBE LTDA</t>
+  </si>
+  <si>
+    <t>57732487000114</t>
+  </si>
+  <si>
+    <t>OVOS CAMPO VERDE LTDA</t>
+  </si>
+  <si>
+    <t>64620731000112</t>
+  </si>
+  <si>
+    <t>R. CEZAR GUSMAO SILVA</t>
+  </si>
+  <si>
+    <t>05022197000183</t>
+  </si>
+  <si>
+    <t>JJF PERFECT SYSTEM SERVICOS DE PINTURA E FUNILARIA LTDA</t>
+  </si>
+  <si>
+    <t>62032111000137</t>
+  </si>
+  <si>
+    <t>IM PRODUTOS AGROPECUARIOS LTDA</t>
+  </si>
+  <si>
+    <t>63861056000150</t>
+  </si>
+  <si>
+    <t>DAVID RIBEIRO DE MELO</t>
+  </si>
+  <si>
+    <t>29068001000150</t>
+  </si>
+  <si>
+    <t>ALENCAR DE JESUS DA SILVA MELLO</t>
+  </si>
+  <si>
+    <t>63532856000128</t>
+  </si>
+  <si>
+    <t>L A DE A COSTA</t>
+  </si>
+  <si>
+    <t>60567946000166</t>
+  </si>
+  <si>
+    <t>R3 COMERCIO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>34094470000183</t>
+  </si>
+  <si>
+    <t>ALMEIDA MARTINS SERVICOS E PECAS LTDA</t>
+  </si>
+  <si>
+    <t>22868609000110</t>
+  </si>
+  <si>
+    <t>41525062000102</t>
+  </si>
+  <si>
+    <t>HOESA GLOBAL LTDA</t>
+  </si>
+  <si>
+    <t>25285209000170</t>
+  </si>
+  <si>
+    <t>HEILER ALMEIDA VIEIRA</t>
+  </si>
+  <si>
+    <t>46274283000160</t>
+  </si>
+  <si>
+    <t>KELLEN RAMOS COSTA LTDA</t>
+  </si>
+  <si>
+    <t>26328271000164</t>
+  </si>
+  <si>
+    <t>FR CONSTRUCOES LTDA</t>
+  </si>
+  <si>
+    <t>31945902000124</t>
+  </si>
+  <si>
+    <t>GIRASSOL PRODUTOS DE PESCA E IMPORTADOS LTDA</t>
+  </si>
+  <si>
+    <t>34731890000123</t>
+  </si>
+  <si>
+    <t>ELIAS CASTILHO DA SILVA</t>
+  </si>
+  <si>
+    <t>42960073000175</t>
+  </si>
+  <si>
+    <t>GAMERO ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>64539617000162</t>
+  </si>
+  <si>
+    <t>ABN PROTEGE REGIONAL SANTANA LTDA</t>
+  </si>
+  <si>
+    <t>58367668000151</t>
+  </si>
+  <si>
+    <t>HORIZONWARE SOLUCOES TECNOLOGICAS LTDA</t>
+  </si>
+  <si>
+    <t>48214395000151</t>
+  </si>
+  <si>
+    <t>CM SERVICOS E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>56173868000148</t>
+  </si>
+  <si>
+    <t>MELO - SERVICO DE TERAPIA LTDA</t>
+  </si>
+  <si>
+    <t>17488793000132</t>
+  </si>
+  <si>
+    <t>SILVANIA EMPREENDIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>05405419000147</t>
+  </si>
+  <si>
+    <t>APRIMORA PRESTADORA DE SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>59907781000145</t>
+  </si>
+  <si>
+    <t>MOURA PACHECO LTDA</t>
+  </si>
+  <si>
+    <t>17544367000179</t>
+  </si>
+  <si>
+    <t>IMUNISAN PEST CONTROL LTDA</t>
+  </si>
+  <si>
+    <t>27097353000108</t>
+  </si>
+  <si>
+    <t>SUSANI DOS SANTOS SILVA</t>
+  </si>
+  <si>
+    <t>50842559000137</t>
+  </si>
+  <si>
+    <t>JAIR PELEGRIN JUNIOR</t>
+  </si>
+  <si>
+    <t>14225761000156</t>
+  </si>
+  <si>
+    <t>GUINCHO EXPRESSO REPUBLICA E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>27388695000187</t>
+  </si>
+  <si>
+    <t>ERILANE FERREIRA DE MELO 38534070300</t>
+  </si>
+  <si>
+    <t>54099836000114</t>
+  </si>
+  <si>
+    <t>A. GONCALO DA SILVA LTDA</t>
+  </si>
+  <si>
+    <t>64207068000129</t>
+  </si>
+  <si>
+    <t>ONEZIMO AR LTDA</t>
+  </si>
+  <si>
+    <t>28468225000196</t>
+  </si>
+  <si>
+    <t>NELCIR JOAO POLINSKI SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>24144952000147</t>
+  </si>
+  <si>
+    <t>OPES PRODUCOES E COBRANCAS LTDA</t>
+  </si>
+  <si>
+    <t>52149083000189</t>
+  </si>
+  <si>
+    <t>OTICA OLHAR MAIS COMERCIO DE OPTICAS LTDA.</t>
+  </si>
+  <si>
+    <t>11898957000113</t>
+  </si>
+  <si>
+    <t>COMETINHA TORQUATO TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>48465622000111</t>
+  </si>
+  <si>
+    <t>LULA EMBREAGENS COMERCIO E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>32005963000174</t>
+  </si>
+  <si>
+    <t>ALCANCE LOCAL MARKETING DIGITAL E PUBLICIDADE LTDA</t>
+  </si>
+  <si>
+    <t>50244611000153</t>
+  </si>
+  <si>
+    <t>LUCIANO P SILVA LTDA</t>
+  </si>
+  <si>
+    <t>37131319000166</t>
+  </si>
+  <si>
+    <t>MINEIROS VEICULOS LTDA</t>
+  </si>
+  <si>
+    <t>44376460000194</t>
+  </si>
+  <si>
+    <t>JM TAPETES PERSONALIZADOS LTDA</t>
+  </si>
+  <si>
+    <t>60664247000134</t>
+  </si>
+  <si>
+    <t>MARXSUELL FERNANDES SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>58550093000108</t>
+  </si>
+  <si>
+    <t>MATHEUS FERNANDES RIBEIRO CAMACAM LTDA</t>
+  </si>
+  <si>
+    <t>53455872000100</t>
+  </si>
+  <si>
+    <t>OPTICA PAJEU LTDA</t>
+  </si>
+  <si>
+    <t>64938502000140</t>
+  </si>
+  <si>
+    <t>ESTETICA AVANCADA ESPACO VOCE LTDA</t>
+  </si>
+  <si>
+    <t>36667580000112</t>
+  </si>
+  <si>
+    <t>GRAFICA MIXTURA LTDA</t>
+  </si>
+  <si>
+    <t>63950895000145</t>
+  </si>
+  <si>
+    <t>JULIANA SIQUEIRA FELIPE LTDA</t>
+  </si>
+  <si>
+    <t>64865100000163</t>
+  </si>
+  <si>
+    <t>SAFIRA LIMPEZAS LTDA</t>
+  </si>
+  <si>
+    <t>64830648000178</t>
+  </si>
+  <si>
+    <t>MARIA DO LIVRAMENTO MENEZES FLORENCIO</t>
+  </si>
+  <si>
+    <t>30643196000101</t>
+  </si>
+  <si>
+    <t>ROBSON PEREIRA DA SILVA EMPILHADEIRA</t>
+  </si>
+  <si>
+    <t>Contrato Social da empresa completo, atualizado e devidamente registrado no orgao competente.&lt;br&gt;&lt;br&gt;Caso a representacao seja em conjunto sera preciso encaminhar a procuracao com poderes para abrir e movimentar contas, o documento deve ser assinado pelos representantes legais nomeados no contrato social, assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF, para validacao das assinaturas e protocolo de autenticidade.</t>
   </si>
 </sst>
 </file>
@@ -2244,10 +2637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
-  <dimension ref="A1:G277"/>
+  <dimension ref="A1:G342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="A277" sqref="A277"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="A342" sqref="A342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,7 +2691,7 @@
         <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2364,10 +2757,10 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" t="s">
-        <v>443</v>
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2433,7 +2826,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -4017,7 +4410,7 @@
         <v>10</v>
       </c>
       <c r="F77" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -5285,7 +5678,7 @@
         <v>113</v>
       </c>
       <c r="G132" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -6742,10 +7135,10 @@
         <v>46057</v>
       </c>
       <c r="B196" t="s">
+        <v>444</v>
+      </c>
+      <c r="C196" t="s">
         <v>445</v>
-      </c>
-      <c r="C196" t="s">
-        <v>446</v>
       </c>
       <c r="D196" t="s">
         <v>60</v>
@@ -6765,10 +7158,10 @@
         <v>46057</v>
       </c>
       <c r="B197" t="s">
+        <v>446</v>
+      </c>
+      <c r="C197" t="s">
         <v>447</v>
-      </c>
-      <c r="C197" t="s">
-        <v>448</v>
       </c>
       <c r="D197" t="s">
         <v>15</v>
@@ -6777,7 +7170,7 @@
         <v>7</v>
       </c>
       <c r="F197" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G197">
         <v>0</v>
@@ -6788,10 +7181,10 @@
         <v>46057</v>
       </c>
       <c r="B198" t="s">
+        <v>448</v>
+      </c>
+      <c r="C198" t="s">
         <v>449</v>
-      </c>
-      <c r="C198" t="s">
-        <v>450</v>
       </c>
       <c r="D198" t="s">
         <v>170</v>
@@ -6811,10 +7204,10 @@
         <v>46057</v>
       </c>
       <c r="B199" t="s">
+        <v>450</v>
+      </c>
+      <c r="C199" t="s">
         <v>451</v>
-      </c>
-      <c r="C199" t="s">
-        <v>452</v>
       </c>
       <c r="D199" t="s">
         <v>110</v>
@@ -6834,10 +7227,10 @@
         <v>46057</v>
       </c>
       <c r="B200" t="s">
+        <v>452</v>
+      </c>
+      <c r="C200" t="s">
         <v>453</v>
-      </c>
-      <c r="C200" t="s">
-        <v>454</v>
       </c>
       <c r="D200" t="s">
         <v>19</v>
@@ -6857,10 +7250,10 @@
         <v>46057</v>
       </c>
       <c r="B201" t="s">
+        <v>454</v>
+      </c>
+      <c r="C201" t="s">
         <v>455</v>
-      </c>
-      <c r="C201" t="s">
-        <v>456</v>
       </c>
       <c r="D201" t="s">
         <v>15</v>
@@ -6869,7 +7262,7 @@
         <v>8</v>
       </c>
       <c r="F201" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G201">
         <v>0</v>
@@ -6880,10 +7273,10 @@
         <v>46057</v>
       </c>
       <c r="B202" t="s">
+        <v>456</v>
+      </c>
+      <c r="C202" t="s">
         <v>457</v>
-      </c>
-      <c r="C202" t="s">
-        <v>458</v>
       </c>
       <c r="D202" t="s">
         <v>86</v>
@@ -6903,10 +7296,10 @@
         <v>46057</v>
       </c>
       <c r="B203" t="s">
+        <v>458</v>
+      </c>
+      <c r="C203" t="s">
         <v>459</v>
-      </c>
-      <c r="C203" t="s">
-        <v>460</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -6926,10 +7319,10 @@
         <v>46057</v>
       </c>
       <c r="B204" t="s">
+        <v>460</v>
+      </c>
+      <c r="C204" t="s">
         <v>461</v>
-      </c>
-      <c r="C204" t="s">
-        <v>462</v>
       </c>
       <c r="D204" t="s">
         <v>86</v>
@@ -6949,10 +7342,10 @@
         <v>46057</v>
       </c>
       <c r="B205" t="s">
+        <v>462</v>
+      </c>
+      <c r="C205" t="s">
         <v>463</v>
-      </c>
-      <c r="C205" t="s">
-        <v>464</v>
       </c>
       <c r="D205" t="s">
         <v>76</v>
@@ -6972,10 +7365,10 @@
         <v>46057</v>
       </c>
       <c r="B206" t="s">
+        <v>464</v>
+      </c>
+      <c r="C206" t="s">
         <v>465</v>
-      </c>
-      <c r="C206" t="s">
-        <v>466</v>
       </c>
       <c r="D206" t="s">
         <v>15</v>
@@ -6984,7 +7377,7 @@
         <v>7</v>
       </c>
       <c r="F206" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G206">
         <v>0</v>
@@ -6995,10 +7388,10 @@
         <v>46057</v>
       </c>
       <c r="B207" t="s">
+        <v>466</v>
+      </c>
+      <c r="C207" t="s">
         <v>467</v>
-      </c>
-      <c r="C207" t="s">
-        <v>468</v>
       </c>
       <c r="D207" t="s">
         <v>9</v>
@@ -7018,10 +7411,10 @@
         <v>46057</v>
       </c>
       <c r="B208" t="s">
+        <v>468</v>
+      </c>
+      <c r="C208" t="s">
         <v>469</v>
-      </c>
-      <c r="C208" t="s">
-        <v>470</v>
       </c>
       <c r="D208" t="s">
         <v>14</v>
@@ -7030,7 +7423,7 @@
         <v>8</v>
       </c>
       <c r="F208" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G208">
         <v>0</v>
@@ -7041,10 +7434,10 @@
         <v>46057</v>
       </c>
       <c r="B209" t="s">
+        <v>470</v>
+      </c>
+      <c r="C209" t="s">
         <v>471</v>
-      </c>
-      <c r="C209" t="s">
-        <v>472</v>
       </c>
       <c r="D209" t="s">
         <v>18</v>
@@ -7064,10 +7457,10 @@
         <v>46057</v>
       </c>
       <c r="B210" t="s">
+        <v>472</v>
+      </c>
+      <c r="C210" t="s">
         <v>473</v>
-      </c>
-      <c r="C210" t="s">
-        <v>474</v>
       </c>
       <c r="D210" t="s">
         <v>15</v>
@@ -7076,7 +7469,7 @@
         <v>7</v>
       </c>
       <c r="F210" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G210">
         <v>0</v>
@@ -7087,10 +7480,10 @@
         <v>46057</v>
       </c>
       <c r="B211" t="s">
+        <v>474</v>
+      </c>
+      <c r="C211" t="s">
         <v>475</v>
-      </c>
-      <c r="C211" t="s">
-        <v>476</v>
       </c>
       <c r="D211" t="s">
         <v>73</v>
@@ -7110,10 +7503,10 @@
         <v>46057</v>
       </c>
       <c r="B212" t="s">
+        <v>476</v>
+      </c>
+      <c r="C212" t="s">
         <v>477</v>
-      </c>
-      <c r="C212" t="s">
-        <v>478</v>
       </c>
       <c r="D212" t="s">
         <v>70</v>
@@ -7122,7 +7515,7 @@
         <v>7</v>
       </c>
       <c r="F212" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G212">
         <v>0</v>
@@ -7133,10 +7526,10 @@
         <v>46057</v>
       </c>
       <c r="B213" t="s">
+        <v>478</v>
+      </c>
+      <c r="C213" t="s">
         <v>479</v>
-      </c>
-      <c r="C213" t="s">
-        <v>480</v>
       </c>
       <c r="D213" t="s">
         <v>14</v>
@@ -7179,10 +7572,10 @@
         <v>46057</v>
       </c>
       <c r="B215" t="s">
+        <v>480</v>
+      </c>
+      <c r="C215" t="s">
         <v>481</v>
-      </c>
-      <c r="C215" t="s">
-        <v>482</v>
       </c>
       <c r="D215" t="s">
         <v>16</v>
@@ -7202,10 +7595,10 @@
         <v>46057</v>
       </c>
       <c r="B216" t="s">
+        <v>482</v>
+      </c>
+      <c r="C216" t="s">
         <v>483</v>
-      </c>
-      <c r="C216" t="s">
-        <v>484</v>
       </c>
       <c r="D216" t="s">
         <v>14</v>
@@ -7225,10 +7618,10 @@
         <v>46057</v>
       </c>
       <c r="B217" t="s">
+        <v>484</v>
+      </c>
+      <c r="C217" t="s">
         <v>485</v>
-      </c>
-      <c r="C217" t="s">
-        <v>486</v>
       </c>
       <c r="D217" t="s">
         <v>67</v>
@@ -7248,10 +7641,10 @@
         <v>46057</v>
       </c>
       <c r="B218" t="s">
+        <v>486</v>
+      </c>
+      <c r="C218" t="s">
         <v>487</v>
-      </c>
-      <c r="C218" t="s">
-        <v>488</v>
       </c>
       <c r="D218" t="s">
         <v>163</v>
@@ -7271,10 +7664,10 @@
         <v>46057</v>
       </c>
       <c r="B219" t="s">
+        <v>488</v>
+      </c>
+      <c r="C219" t="s">
         <v>489</v>
-      </c>
-      <c r="C219" t="s">
-        <v>490</v>
       </c>
       <c r="D219" t="s">
         <v>170</v>
@@ -7294,10 +7687,10 @@
         <v>46057</v>
       </c>
       <c r="B220" t="s">
+        <v>490</v>
+      </c>
+      <c r="C220" t="s">
         <v>491</v>
-      </c>
-      <c r="C220" t="s">
-        <v>492</v>
       </c>
       <c r="D220" t="s">
         <v>170</v>
@@ -7317,10 +7710,10 @@
         <v>46057</v>
       </c>
       <c r="B221" t="s">
+        <v>492</v>
+      </c>
+      <c r="C221" t="s">
         <v>493</v>
-      </c>
-      <c r="C221" t="s">
-        <v>494</v>
       </c>
       <c r="D221" t="s">
         <v>18</v>
@@ -7340,10 +7733,10 @@
         <v>46057</v>
       </c>
       <c r="B222" t="s">
+        <v>494</v>
+      </c>
+      <c r="C222" t="s">
         <v>495</v>
-      </c>
-      <c r="C222" t="s">
-        <v>496</v>
       </c>
       <c r="D222" t="s">
         <v>14</v>
@@ -7363,10 +7756,10 @@
         <v>46057</v>
       </c>
       <c r="B223" t="s">
+        <v>496</v>
+      </c>
+      <c r="C223" t="s">
         <v>497</v>
-      </c>
-      <c r="C223" t="s">
-        <v>498</v>
       </c>
       <c r="D223" t="s">
         <v>60</v>
@@ -7375,7 +7768,7 @@
         <v>8</v>
       </c>
       <c r="F223" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G223">
         <v>0</v>
@@ -7386,10 +7779,10 @@
         <v>46057</v>
       </c>
       <c r="B224" t="s">
+        <v>498</v>
+      </c>
+      <c r="C224" t="s">
         <v>499</v>
-      </c>
-      <c r="C224" t="s">
-        <v>500</v>
       </c>
       <c r="D224" t="s">
         <v>18</v>
@@ -7409,10 +7802,10 @@
         <v>46057</v>
       </c>
       <c r="B225" t="s">
+        <v>500</v>
+      </c>
+      <c r="C225" t="s">
         <v>501</v>
-      </c>
-      <c r="C225" t="s">
-        <v>502</v>
       </c>
       <c r="D225" t="s">
         <v>73</v>
@@ -7432,10 +7825,10 @@
         <v>46057</v>
       </c>
       <c r="B226" t="s">
+        <v>502</v>
+      </c>
+      <c r="C226" t="s">
         <v>503</v>
-      </c>
-      <c r="C226" t="s">
-        <v>504</v>
       </c>
       <c r="D226" t="s">
         <v>15</v>
@@ -7444,7 +7837,7 @@
         <v>8</v>
       </c>
       <c r="F226" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G226">
         <v>0</v>
@@ -7455,10 +7848,10 @@
         <v>46057</v>
       </c>
       <c r="B227" t="s">
+        <v>504</v>
+      </c>
+      <c r="C227" t="s">
         <v>505</v>
-      </c>
-      <c r="C227" t="s">
-        <v>506</v>
       </c>
       <c r="D227" t="s">
         <v>110</v>
@@ -7478,10 +7871,10 @@
         <v>46057</v>
       </c>
       <c r="B228" t="s">
+        <v>506</v>
+      </c>
+      <c r="C228" t="s">
         <v>507</v>
-      </c>
-      <c r="C228" t="s">
-        <v>508</v>
       </c>
       <c r="D228" t="s">
         <v>73</v>
@@ -7501,10 +7894,10 @@
         <v>46057</v>
       </c>
       <c r="B229" t="s">
+        <v>508</v>
+      </c>
+      <c r="C229" t="s">
         <v>509</v>
-      </c>
-      <c r="C229" t="s">
-        <v>510</v>
       </c>
       <c r="D229" t="s">
         <v>19</v>
@@ -7524,10 +7917,10 @@
         <v>46057</v>
       </c>
       <c r="B230" t="s">
+        <v>510</v>
+      </c>
+      <c r="C230" t="s">
         <v>511</v>
-      </c>
-      <c r="C230" t="s">
-        <v>512</v>
       </c>
       <c r="D230" t="s">
         <v>17</v>
@@ -7547,10 +7940,10 @@
         <v>46057</v>
       </c>
       <c r="B231" t="s">
+        <v>512</v>
+      </c>
+      <c r="C231" t="s">
         <v>513</v>
-      </c>
-      <c r="C231" t="s">
-        <v>514</v>
       </c>
       <c r="D231" t="s">
         <v>12</v>
@@ -7570,10 +7963,10 @@
         <v>46057</v>
       </c>
       <c r="B232" t="s">
+        <v>514</v>
+      </c>
+      <c r="C232" t="s">
         <v>515</v>
-      </c>
-      <c r="C232" t="s">
-        <v>516</v>
       </c>
       <c r="D232" t="s">
         <v>11</v>
@@ -7593,10 +7986,10 @@
         <v>46057</v>
       </c>
       <c r="B233" t="s">
+        <v>516</v>
+      </c>
+      <c r="C233" t="s">
         <v>517</v>
-      </c>
-      <c r="C233" t="s">
-        <v>518</v>
       </c>
       <c r="D233" t="s">
         <v>110</v>
@@ -7616,10 +8009,10 @@
         <v>46057</v>
       </c>
       <c r="B234" t="s">
+        <v>518</v>
+      </c>
+      <c r="C234" t="s">
         <v>519</v>
-      </c>
-      <c r="C234" t="s">
-        <v>520</v>
       </c>
       <c r="D234" t="s">
         <v>9</v>
@@ -7639,10 +8032,10 @@
         <v>46057</v>
       </c>
       <c r="B235" t="s">
+        <v>520</v>
+      </c>
+      <c r="C235" t="s">
         <v>521</v>
-      </c>
-      <c r="C235" t="s">
-        <v>522</v>
       </c>
       <c r="D235" t="s">
         <v>17</v>
@@ -7662,10 +8055,10 @@
         <v>46057</v>
       </c>
       <c r="B236" t="s">
+        <v>522</v>
+      </c>
+      <c r="C236" t="s">
         <v>523</v>
-      </c>
-      <c r="C236" t="s">
-        <v>524</v>
       </c>
       <c r="D236" t="s">
         <v>170</v>
@@ -7685,10 +8078,10 @@
         <v>46057</v>
       </c>
       <c r="B237" t="s">
+        <v>524</v>
+      </c>
+      <c r="C237" t="s">
         <v>525</v>
-      </c>
-      <c r="C237" t="s">
-        <v>526</v>
       </c>
       <c r="D237" t="s">
         <v>16</v>
@@ -7708,10 +8101,10 @@
         <v>46057</v>
       </c>
       <c r="B238" t="s">
+        <v>526</v>
+      </c>
+      <c r="C238" t="s">
         <v>527</v>
-      </c>
-      <c r="C238" t="s">
-        <v>528</v>
       </c>
       <c r="D238" t="s">
         <v>16</v>
@@ -7731,10 +8124,10 @@
         <v>46057</v>
       </c>
       <c r="B239" t="s">
+        <v>528</v>
+      </c>
+      <c r="C239" t="s">
         <v>529</v>
-      </c>
-      <c r="C239" t="s">
-        <v>530</v>
       </c>
       <c r="D239" t="s">
         <v>9</v>
@@ -7754,10 +8147,10 @@
         <v>46057</v>
       </c>
       <c r="B240" t="s">
+        <v>530</v>
+      </c>
+      <c r="C240" t="s">
         <v>531</v>
-      </c>
-      <c r="C240" t="s">
-        <v>532</v>
       </c>
       <c r="D240" t="s">
         <v>12</v>
@@ -7777,10 +8170,10 @@
         <v>46057</v>
       </c>
       <c r="B241" t="s">
+        <v>532</v>
+      </c>
+      <c r="C241" t="s">
         <v>533</v>
-      </c>
-      <c r="C241" t="s">
-        <v>534</v>
       </c>
       <c r="D241" t="s">
         <v>16</v>
@@ -7800,10 +8193,10 @@
         <v>46057</v>
       </c>
       <c r="B242" t="s">
+        <v>534</v>
+      </c>
+      <c r="C242" t="s">
         <v>535</v>
-      </c>
-      <c r="C242" t="s">
-        <v>536</v>
       </c>
       <c r="D242" t="s">
         <v>40</v>
@@ -7814,8 +8207,8 @@
       <c r="F242" t="s">
         <v>51</v>
       </c>
-      <c r="G242">
-        <v>0</v>
+      <c r="G242" t="s">
+        <v>741</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -7823,10 +8216,10 @@
         <v>46057</v>
       </c>
       <c r="B243" t="s">
+        <v>536</v>
+      </c>
+      <c r="C243" t="s">
         <v>537</v>
-      </c>
-      <c r="C243" t="s">
-        <v>538</v>
       </c>
       <c r="D243" t="s">
         <v>14</v>
@@ -7846,10 +8239,10 @@
         <v>46057</v>
       </c>
       <c r="B244" t="s">
+        <v>538</v>
+      </c>
+      <c r="C244" t="s">
         <v>539</v>
-      </c>
-      <c r="C244" t="s">
-        <v>540</v>
       </c>
       <c r="D244" t="s">
         <v>16</v>
@@ -7869,10 +8262,10 @@
         <v>46057</v>
       </c>
       <c r="B245" t="s">
+        <v>540</v>
+      </c>
+      <c r="C245" t="s">
         <v>541</v>
-      </c>
-      <c r="C245" t="s">
-        <v>542</v>
       </c>
       <c r="D245" t="s">
         <v>16</v>
@@ -7892,10 +8285,10 @@
         <v>46057</v>
       </c>
       <c r="B246" t="s">
+        <v>542</v>
+      </c>
+      <c r="C246" t="s">
         <v>543</v>
-      </c>
-      <c r="C246" t="s">
-        <v>544</v>
       </c>
       <c r="D246" t="s">
         <v>18</v>
@@ -7904,7 +8297,7 @@
         <v>8</v>
       </c>
       <c r="F246" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="G246" t="s">
         <v>265</v>
@@ -7915,10 +8308,10 @@
         <v>46057</v>
       </c>
       <c r="B247" t="s">
+        <v>544</v>
+      </c>
+      <c r="C247" t="s">
         <v>545</v>
-      </c>
-      <c r="C247" t="s">
-        <v>546</v>
       </c>
       <c r="D247" t="s">
         <v>15</v>
@@ -7927,7 +8320,7 @@
         <v>8</v>
       </c>
       <c r="F247" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G247">
         <v>0</v>
@@ -7938,10 +8331,10 @@
         <v>46057</v>
       </c>
       <c r="B248" t="s">
+        <v>546</v>
+      </c>
+      <c r="C248" t="s">
         <v>547</v>
-      </c>
-      <c r="C248" t="s">
-        <v>548</v>
       </c>
       <c r="D248" t="s">
         <v>16</v>
@@ -7961,10 +8354,10 @@
         <v>46057</v>
       </c>
       <c r="B249" t="s">
+        <v>548</v>
+      </c>
+      <c r="C249" t="s">
         <v>549</v>
-      </c>
-      <c r="C249" t="s">
-        <v>550</v>
       </c>
       <c r="D249" t="s">
         <v>18</v>
@@ -7984,10 +8377,10 @@
         <v>46057</v>
       </c>
       <c r="B250" t="s">
+        <v>550</v>
+      </c>
+      <c r="C250" t="s">
         <v>551</v>
-      </c>
-      <c r="C250" t="s">
-        <v>552</v>
       </c>
       <c r="D250" t="s">
         <v>14</v>
@@ -8007,10 +8400,10 @@
         <v>46057</v>
       </c>
       <c r="B251" t="s">
+        <v>552</v>
+      </c>
+      <c r="C251" t="s">
         <v>553</v>
-      </c>
-      <c r="C251" t="s">
-        <v>554</v>
       </c>
       <c r="D251" t="s">
         <v>73</v>
@@ -8030,10 +8423,10 @@
         <v>46057</v>
       </c>
       <c r="B252" t="s">
+        <v>554</v>
+      </c>
+      <c r="C252" t="s">
         <v>555</v>
-      </c>
-      <c r="C252" t="s">
-        <v>556</v>
       </c>
       <c r="D252" t="s">
         <v>170</v>
@@ -8053,10 +8446,10 @@
         <v>46057</v>
       </c>
       <c r="B253" t="s">
+        <v>556</v>
+      </c>
+      <c r="C253" t="s">
         <v>557</v>
-      </c>
-      <c r="C253" t="s">
-        <v>558</v>
       </c>
       <c r="D253" t="s">
         <v>60</v>
@@ -8076,10 +8469,10 @@
         <v>46057</v>
       </c>
       <c r="B254" t="s">
+        <v>558</v>
+      </c>
+      <c r="C254" t="s">
         <v>559</v>
-      </c>
-      <c r="C254" t="s">
-        <v>560</v>
       </c>
       <c r="D254" t="s">
         <v>17</v>
@@ -8099,10 +8492,10 @@
         <v>46057</v>
       </c>
       <c r="B255" t="s">
+        <v>560</v>
+      </c>
+      <c r="C255" t="s">
         <v>561</v>
-      </c>
-      <c r="C255" t="s">
-        <v>562</v>
       </c>
       <c r="D255" t="s">
         <v>19</v>
@@ -8122,10 +8515,10 @@
         <v>46057</v>
       </c>
       <c r="B256" t="s">
+        <v>562</v>
+      </c>
+      <c r="C256" t="s">
         <v>563</v>
-      </c>
-      <c r="C256" t="s">
-        <v>564</v>
       </c>
       <c r="D256" t="s">
         <v>152</v>
@@ -8145,10 +8538,10 @@
         <v>46057</v>
       </c>
       <c r="B257" t="s">
+        <v>564</v>
+      </c>
+      <c r="C257" t="s">
         <v>565</v>
-      </c>
-      <c r="C257" t="s">
-        <v>566</v>
       </c>
       <c r="D257" t="s">
         <v>73</v>
@@ -8168,10 +8561,10 @@
         <v>46057</v>
       </c>
       <c r="B258" t="s">
+        <v>566</v>
+      </c>
+      <c r="C258" t="s">
         <v>567</v>
-      </c>
-      <c r="C258" t="s">
-        <v>568</v>
       </c>
       <c r="D258" t="s">
         <v>14</v>
@@ -8191,10 +8584,10 @@
         <v>46057</v>
       </c>
       <c r="B259" t="s">
+        <v>568</v>
+      </c>
+      <c r="C259" t="s">
         <v>569</v>
-      </c>
-      <c r="C259" t="s">
-        <v>570</v>
       </c>
       <c r="D259" t="s">
         <v>14</v>
@@ -8214,10 +8607,10 @@
         <v>46057</v>
       </c>
       <c r="B260" t="s">
+        <v>570</v>
+      </c>
+      <c r="C260" t="s">
         <v>571</v>
-      </c>
-      <c r="C260" t="s">
-        <v>572</v>
       </c>
       <c r="D260" t="s">
         <v>110</v>
@@ -8237,10 +8630,10 @@
         <v>46057</v>
       </c>
       <c r="B261" t="s">
+        <v>572</v>
+      </c>
+      <c r="C261" t="s">
         <v>573</v>
-      </c>
-      <c r="C261" t="s">
-        <v>574</v>
       </c>
       <c r="D261" t="s">
         <v>170</v>
@@ -8260,13 +8653,13 @@
         <v>46057</v>
       </c>
       <c r="B262" t="s">
+        <v>574</v>
+      </c>
+      <c r="C262" t="s">
         <v>575</v>
       </c>
-      <c r="C262" t="s">
+      <c r="D262" t="s">
         <v>576</v>
-      </c>
-      <c r="D262" t="s">
-        <v>577</v>
       </c>
       <c r="E262" t="s">
         <v>191</v>
@@ -8283,10 +8676,10 @@
         <v>46057</v>
       </c>
       <c r="B263" t="s">
+        <v>577</v>
+      </c>
+      <c r="C263" t="s">
         <v>578</v>
-      </c>
-      <c r="C263" t="s">
-        <v>579</v>
       </c>
       <c r="D263" t="s">
         <v>170</v>
@@ -8306,10 +8699,10 @@
         <v>46057</v>
       </c>
       <c r="B264" t="s">
+        <v>579</v>
+      </c>
+      <c r="C264" t="s">
         <v>580</v>
-      </c>
-      <c r="C264" t="s">
-        <v>581</v>
       </c>
       <c r="D264" t="s">
         <v>11</v>
@@ -8329,10 +8722,10 @@
         <v>46057</v>
       </c>
       <c r="B265" t="s">
+        <v>581</v>
+      </c>
+      <c r="C265" t="s">
         <v>582</v>
-      </c>
-      <c r="C265" t="s">
-        <v>583</v>
       </c>
       <c r="D265" t="s">
         <v>40</v>
@@ -8352,10 +8745,10 @@
         <v>46057</v>
       </c>
       <c r="B266" t="s">
+        <v>583</v>
+      </c>
+      <c r="C266" t="s">
         <v>584</v>
-      </c>
-      <c r="C266" t="s">
-        <v>585</v>
       </c>
       <c r="D266" t="s">
         <v>152</v>
@@ -8375,13 +8768,13 @@
         <v>46057</v>
       </c>
       <c r="B267" t="s">
+        <v>585</v>
+      </c>
+      <c r="C267" t="s">
         <v>586</v>
       </c>
-      <c r="C267" t="s">
+      <c r="D267" t="s">
         <v>587</v>
-      </c>
-      <c r="D267" t="s">
-        <v>588</v>
       </c>
       <c r="E267" t="s">
         <v>119</v>
@@ -8398,10 +8791,10 @@
         <v>46057</v>
       </c>
       <c r="B268" t="s">
+        <v>588</v>
+      </c>
+      <c r="C268" t="s">
         <v>589</v>
-      </c>
-      <c r="C268" t="s">
-        <v>590</v>
       </c>
       <c r="D268" t="s">
         <v>200</v>
@@ -8421,10 +8814,10 @@
         <v>46057</v>
       </c>
       <c r="B269" t="s">
+        <v>590</v>
+      </c>
+      <c r="C269" t="s">
         <v>591</v>
-      </c>
-      <c r="C269" t="s">
-        <v>592</v>
       </c>
       <c r="D269" t="s">
         <v>12</v>
@@ -8444,10 +8837,10 @@
         <v>46058</v>
       </c>
       <c r="B270" t="s">
+        <v>592</v>
+      </c>
+      <c r="C270" t="s">
         <v>593</v>
-      </c>
-      <c r="C270" t="s">
-        <v>594</v>
       </c>
       <c r="D270" t="s">
         <v>16</v>
@@ -8467,10 +8860,10 @@
         <v>46058</v>
       </c>
       <c r="B271" t="s">
+        <v>594</v>
+      </c>
+      <c r="C271" t="s">
         <v>595</v>
-      </c>
-      <c r="C271" t="s">
-        <v>596</v>
       </c>
       <c r="D271" t="s">
         <v>67</v>
@@ -8490,10 +8883,10 @@
         <v>46058</v>
       </c>
       <c r="B272" t="s">
+        <v>596</v>
+      </c>
+      <c r="C272" t="s">
         <v>597</v>
-      </c>
-      <c r="C272" t="s">
-        <v>598</v>
       </c>
       <c r="D272" t="s">
         <v>11</v>
@@ -8513,13 +8906,13 @@
         <v>46058</v>
       </c>
       <c r="B273" t="s">
+        <v>598</v>
+      </c>
+      <c r="C273" t="s">
         <v>599</v>
       </c>
-      <c r="C273" t="s">
+      <c r="D273" t="s">
         <v>600</v>
-      </c>
-      <c r="D273" t="s">
-        <v>601</v>
       </c>
       <c r="F273" t="s">
         <v>21</v>
@@ -8533,10 +8926,10 @@
         <v>46058</v>
       </c>
       <c r="B274" t="s">
+        <v>601</v>
+      </c>
+      <c r="C274" t="s">
         <v>602</v>
-      </c>
-      <c r="C274" t="s">
-        <v>603</v>
       </c>
       <c r="D274" t="s">
         <v>152</v>
@@ -8556,10 +8949,10 @@
         <v>46058</v>
       </c>
       <c r="B275" t="s">
+        <v>603</v>
+      </c>
+      <c r="C275" t="s">
         <v>604</v>
-      </c>
-      <c r="C275" t="s">
-        <v>605</v>
       </c>
       <c r="D275" t="s">
         <v>19</v>
@@ -8579,10 +8972,10 @@
         <v>46058</v>
       </c>
       <c r="B276" t="s">
+        <v>605</v>
+      </c>
+      <c r="C276" t="s">
         <v>606</v>
-      </c>
-      <c r="C276" t="s">
-        <v>607</v>
       </c>
       <c r="D276" t="s">
         <v>16</v>
@@ -8602,10 +8995,10 @@
         <v>46058</v>
       </c>
       <c r="B277" t="s">
+        <v>607</v>
+      </c>
+      <c r="C277" t="s">
         <v>608</v>
-      </c>
-      <c r="C277" t="s">
-        <v>609</v>
       </c>
       <c r="D277" t="s">
         <v>17</v>
@@ -8617,6 +9010,1495 @@
         <v>21</v>
       </c>
       <c r="G277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B278" t="s">
+        <v>610</v>
+      </c>
+      <c r="C278" t="s">
+        <v>611</v>
+      </c>
+      <c r="D278" t="s">
+        <v>612</v>
+      </c>
+      <c r="E278" t="s">
+        <v>613</v>
+      </c>
+      <c r="F278" t="s">
+        <v>21</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B279" t="s">
+        <v>614</v>
+      </c>
+      <c r="C279" t="s">
+        <v>615</v>
+      </c>
+      <c r="D279" t="s">
+        <v>612</v>
+      </c>
+      <c r="E279" t="s">
+        <v>613</v>
+      </c>
+      <c r="F279" t="s">
+        <v>21</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B280" t="s">
+        <v>616</v>
+      </c>
+      <c r="C280" t="s">
+        <v>617</v>
+      </c>
+      <c r="D280" t="s">
+        <v>612</v>
+      </c>
+      <c r="E280" t="s">
+        <v>613</v>
+      </c>
+      <c r="F280" t="s">
+        <v>21</v>
+      </c>
+      <c r="G280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B281" t="s">
+        <v>618</v>
+      </c>
+      <c r="C281" t="s">
+        <v>619</v>
+      </c>
+      <c r="D281" t="s">
+        <v>70</v>
+      </c>
+      <c r="E281" t="s">
+        <v>8</v>
+      </c>
+      <c r="F281" t="s">
+        <v>21</v>
+      </c>
+      <c r="G281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B282" t="s">
+        <v>620</v>
+      </c>
+      <c r="C282" t="s">
+        <v>621</v>
+      </c>
+      <c r="D282" t="s">
+        <v>18</v>
+      </c>
+      <c r="E282" t="s">
+        <v>8</v>
+      </c>
+      <c r="F282" t="s">
+        <v>21</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B283" t="s">
+        <v>622</v>
+      </c>
+      <c r="C283" t="s">
+        <v>623</v>
+      </c>
+      <c r="D283" t="s">
+        <v>11</v>
+      </c>
+      <c r="E283" t="s">
+        <v>8</v>
+      </c>
+      <c r="F283" t="s">
+        <v>21</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B284" t="s">
+        <v>624</v>
+      </c>
+      <c r="C284" t="s">
+        <v>625</v>
+      </c>
+      <c r="D284" t="s">
+        <v>16</v>
+      </c>
+      <c r="E284" t="s">
+        <v>8</v>
+      </c>
+      <c r="F284" t="s">
+        <v>21</v>
+      </c>
+      <c r="G284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B285" t="s">
+        <v>626</v>
+      </c>
+      <c r="C285" t="s">
+        <v>627</v>
+      </c>
+      <c r="D285" t="s">
+        <v>211</v>
+      </c>
+      <c r="E285" t="s">
+        <v>10</v>
+      </c>
+      <c r="F285" t="s">
+        <v>21</v>
+      </c>
+      <c r="G285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B286" t="s">
+        <v>628</v>
+      </c>
+      <c r="C286" t="s">
+        <v>629</v>
+      </c>
+      <c r="D286" t="s">
+        <v>67</v>
+      </c>
+      <c r="E286" t="s">
+        <v>10</v>
+      </c>
+      <c r="F286" t="s">
+        <v>52</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B287" t="s">
+        <v>630</v>
+      </c>
+      <c r="C287" t="s">
+        <v>631</v>
+      </c>
+      <c r="D287" t="s">
+        <v>14</v>
+      </c>
+      <c r="E287" t="s">
+        <v>8</v>
+      </c>
+      <c r="F287" t="s">
+        <v>21</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B288" t="s">
+        <v>632</v>
+      </c>
+      <c r="C288" t="s">
+        <v>633</v>
+      </c>
+      <c r="D288" t="s">
+        <v>9</v>
+      </c>
+      <c r="E288" t="s">
+        <v>7</v>
+      </c>
+      <c r="F288" t="s">
+        <v>21</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B289" t="s">
+        <v>634</v>
+      </c>
+      <c r="C289" t="s">
+        <v>635</v>
+      </c>
+      <c r="D289" t="s">
+        <v>19</v>
+      </c>
+      <c r="E289" t="s">
+        <v>10</v>
+      </c>
+      <c r="F289" t="s">
+        <v>21</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B290" t="s">
+        <v>636</v>
+      </c>
+      <c r="C290" t="s">
+        <v>637</v>
+      </c>
+      <c r="D290" t="s">
+        <v>110</v>
+      </c>
+      <c r="E290" t="s">
+        <v>7</v>
+      </c>
+      <c r="F290" t="s">
+        <v>51</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B291" t="s">
+        <v>638</v>
+      </c>
+      <c r="C291" t="s">
+        <v>639</v>
+      </c>
+      <c r="D291" t="s">
+        <v>14</v>
+      </c>
+      <c r="E291" t="s">
+        <v>8</v>
+      </c>
+      <c r="F291" t="s">
+        <v>113</v>
+      </c>
+      <c r="G291" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B292" t="s">
+        <v>640</v>
+      </c>
+      <c r="C292" t="s">
+        <v>641</v>
+      </c>
+      <c r="D292" t="s">
+        <v>76</v>
+      </c>
+      <c r="E292" t="s">
+        <v>10</v>
+      </c>
+      <c r="F292" t="s">
+        <v>21</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B293" t="s">
+        <v>642</v>
+      </c>
+      <c r="C293" t="s">
+        <v>643</v>
+      </c>
+      <c r="D293" t="s">
+        <v>16</v>
+      </c>
+      <c r="E293" t="s">
+        <v>8</v>
+      </c>
+      <c r="F293" t="s">
+        <v>52</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B294" t="s">
+        <v>644</v>
+      </c>
+      <c r="C294" t="s">
+        <v>645</v>
+      </c>
+      <c r="D294" t="s">
+        <v>12</v>
+      </c>
+      <c r="E294" t="s">
+        <v>8</v>
+      </c>
+      <c r="F294" t="s">
+        <v>21</v>
+      </c>
+      <c r="G294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B295" t="s">
+        <v>646</v>
+      </c>
+      <c r="C295" t="s">
+        <v>647</v>
+      </c>
+      <c r="D295" t="s">
+        <v>19</v>
+      </c>
+      <c r="E295" t="s">
+        <v>10</v>
+      </c>
+      <c r="F295" t="s">
+        <v>21</v>
+      </c>
+      <c r="G295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B296" t="s">
+        <v>648</v>
+      </c>
+      <c r="C296" t="s">
+        <v>649</v>
+      </c>
+      <c r="D296" t="s">
+        <v>18</v>
+      </c>
+      <c r="E296" t="s">
+        <v>7</v>
+      </c>
+      <c r="F296" t="s">
+        <v>52</v>
+      </c>
+      <c r="G296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B297" t="s">
+        <v>650</v>
+      </c>
+      <c r="C297" t="s">
+        <v>651</v>
+      </c>
+      <c r="D297" t="s">
+        <v>17</v>
+      </c>
+      <c r="E297" t="s">
+        <v>13</v>
+      </c>
+      <c r="F297" t="s">
+        <v>51</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B298" t="s">
+        <v>652</v>
+      </c>
+      <c r="C298" t="s">
+        <v>653</v>
+      </c>
+      <c r="D298" t="s">
+        <v>19</v>
+      </c>
+      <c r="E298" t="s">
+        <v>8</v>
+      </c>
+      <c r="F298" t="s">
+        <v>51</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B299" t="s">
+        <v>654</v>
+      </c>
+      <c r="C299" t="s">
+        <v>655</v>
+      </c>
+      <c r="D299" t="s">
+        <v>11</v>
+      </c>
+      <c r="E299" t="s">
+        <v>8</v>
+      </c>
+      <c r="F299" t="s">
+        <v>21</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B300" t="s">
+        <v>656</v>
+      </c>
+      <c r="C300" t="s">
+        <v>657</v>
+      </c>
+      <c r="D300" t="s">
+        <v>211</v>
+      </c>
+      <c r="E300" t="s">
+        <v>10</v>
+      </c>
+      <c r="F300" t="s">
+        <v>51</v>
+      </c>
+      <c r="G300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B301" t="s">
+        <v>658</v>
+      </c>
+      <c r="C301" t="s">
+        <v>659</v>
+      </c>
+      <c r="D301" t="s">
+        <v>12</v>
+      </c>
+      <c r="E301" t="s">
+        <v>8</v>
+      </c>
+      <c r="F301" t="s">
+        <v>21</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B302" t="s">
+        <v>660</v>
+      </c>
+      <c r="C302" t="s">
+        <v>661</v>
+      </c>
+      <c r="D302" t="s">
+        <v>16</v>
+      </c>
+      <c r="E302" t="s">
+        <v>8</v>
+      </c>
+      <c r="F302" t="s">
+        <v>51</v>
+      </c>
+      <c r="G302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B303" t="s">
+        <v>662</v>
+      </c>
+      <c r="C303" t="s">
+        <v>174</v>
+      </c>
+      <c r="D303" t="s">
+        <v>18</v>
+      </c>
+      <c r="E303" t="s">
+        <v>8</v>
+      </c>
+      <c r="F303" t="s">
+        <v>51</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B304" t="s">
+        <v>663</v>
+      </c>
+      <c r="C304" t="s">
+        <v>664</v>
+      </c>
+      <c r="D304" t="s">
+        <v>9</v>
+      </c>
+      <c r="E304" t="s">
+        <v>7</v>
+      </c>
+      <c r="F304" t="s">
+        <v>51</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B305" t="s">
+        <v>665</v>
+      </c>
+      <c r="C305" t="s">
+        <v>666</v>
+      </c>
+      <c r="D305" t="s">
+        <v>163</v>
+      </c>
+      <c r="E305" t="s">
+        <v>8</v>
+      </c>
+      <c r="F305" t="s">
+        <v>21</v>
+      </c>
+      <c r="G305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B306" t="s">
+        <v>667</v>
+      </c>
+      <c r="C306" t="s">
+        <v>668</v>
+      </c>
+      <c r="D306" t="s">
+        <v>18</v>
+      </c>
+      <c r="E306" t="s">
+        <v>8</v>
+      </c>
+      <c r="F306" t="s">
+        <v>21</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B307" t="s">
+        <v>669</v>
+      </c>
+      <c r="C307" t="s">
+        <v>670</v>
+      </c>
+      <c r="D307" t="s">
+        <v>24</v>
+      </c>
+      <c r="E307" t="s">
+        <v>8</v>
+      </c>
+      <c r="F307" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B308" t="s">
+        <v>671</v>
+      </c>
+      <c r="C308" t="s">
+        <v>672</v>
+      </c>
+      <c r="D308" t="s">
+        <v>18</v>
+      </c>
+      <c r="E308" t="s">
+        <v>8</v>
+      </c>
+      <c r="F308" t="s">
+        <v>21</v>
+      </c>
+      <c r="G308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B309" t="s">
+        <v>673</v>
+      </c>
+      <c r="C309" t="s">
+        <v>674</v>
+      </c>
+      <c r="D309" t="s">
+        <v>16</v>
+      </c>
+      <c r="E309" t="s">
+        <v>8</v>
+      </c>
+      <c r="F309" t="s">
+        <v>21</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B310" t="s">
+        <v>675</v>
+      </c>
+      <c r="C310" t="s">
+        <v>676</v>
+      </c>
+      <c r="D310" t="s">
+        <v>211</v>
+      </c>
+      <c r="E310" t="s">
+        <v>10</v>
+      </c>
+      <c r="F310" t="s">
+        <v>21</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B311" t="s">
+        <v>677</v>
+      </c>
+      <c r="C311" t="s">
+        <v>678</v>
+      </c>
+      <c r="D311" t="s">
+        <v>19</v>
+      </c>
+      <c r="E311" t="s">
+        <v>10</v>
+      </c>
+      <c r="F311" t="s">
+        <v>51</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B312" t="s">
+        <v>679</v>
+      </c>
+      <c r="C312" t="s">
+        <v>680</v>
+      </c>
+      <c r="D312" t="s">
+        <v>18</v>
+      </c>
+      <c r="E312" t="s">
+        <v>8</v>
+      </c>
+      <c r="F312" t="s">
+        <v>21</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B313" t="s">
+        <v>681</v>
+      </c>
+      <c r="C313" t="s">
+        <v>682</v>
+      </c>
+      <c r="D313" t="s">
+        <v>163</v>
+      </c>
+      <c r="E313" t="s">
+        <v>8</v>
+      </c>
+      <c r="F313" t="s">
+        <v>51</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B314" t="s">
+        <v>683</v>
+      </c>
+      <c r="C314" t="s">
+        <v>684</v>
+      </c>
+      <c r="D314" t="s">
+        <v>15</v>
+      </c>
+      <c r="E314" t="s">
+        <v>8</v>
+      </c>
+      <c r="F314" t="s">
+        <v>21</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B315" t="s">
+        <v>685</v>
+      </c>
+      <c r="C315" t="s">
+        <v>686</v>
+      </c>
+      <c r="D315" t="s">
+        <v>18</v>
+      </c>
+      <c r="E315" t="s">
+        <v>8</v>
+      </c>
+      <c r="F315" t="s">
+        <v>21</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B316" t="s">
+        <v>687</v>
+      </c>
+      <c r="C316" t="s">
+        <v>688</v>
+      </c>
+      <c r="D316" t="s">
+        <v>86</v>
+      </c>
+      <c r="E316" t="s">
+        <v>13</v>
+      </c>
+      <c r="F316" t="s">
+        <v>21</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B317" t="s">
+        <v>689</v>
+      </c>
+      <c r="C317" t="s">
+        <v>690</v>
+      </c>
+      <c r="D317" t="s">
+        <v>18</v>
+      </c>
+      <c r="E317" t="s">
+        <v>8</v>
+      </c>
+      <c r="F317" t="s">
+        <v>21</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B318" t="s">
+        <v>691</v>
+      </c>
+      <c r="C318" t="s">
+        <v>692</v>
+      </c>
+      <c r="D318" t="s">
+        <v>11</v>
+      </c>
+      <c r="E318" t="s">
+        <v>8</v>
+      </c>
+      <c r="F318" t="s">
+        <v>21</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B319" t="s">
+        <v>693</v>
+      </c>
+      <c r="C319" t="s">
+        <v>694</v>
+      </c>
+      <c r="D319" t="s">
+        <v>15</v>
+      </c>
+      <c r="E319" t="s">
+        <v>8</v>
+      </c>
+      <c r="F319" t="s">
+        <v>51</v>
+      </c>
+      <c r="G319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B320" t="s">
+        <v>695</v>
+      </c>
+      <c r="C320" t="s">
+        <v>696</v>
+      </c>
+      <c r="D320" t="s">
+        <v>19</v>
+      </c>
+      <c r="E320" t="s">
+        <v>8</v>
+      </c>
+      <c r="F320" t="s">
+        <v>21</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B321" t="s">
+        <v>697</v>
+      </c>
+      <c r="C321" t="s">
+        <v>698</v>
+      </c>
+      <c r="D321" t="s">
+        <v>67</v>
+      </c>
+      <c r="E321" t="s">
+        <v>10</v>
+      </c>
+      <c r="F321" t="s">
+        <v>21</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B322" t="s">
+        <v>699</v>
+      </c>
+      <c r="C322" t="s">
+        <v>700</v>
+      </c>
+      <c r="D322" t="s">
+        <v>70</v>
+      </c>
+      <c r="E322" t="s">
+        <v>8</v>
+      </c>
+      <c r="F322" t="s">
+        <v>21</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B323" t="s">
+        <v>701</v>
+      </c>
+      <c r="C323" t="s">
+        <v>702</v>
+      </c>
+      <c r="D323" t="s">
+        <v>70</v>
+      </c>
+      <c r="E323" t="s">
+        <v>8</v>
+      </c>
+      <c r="F323" t="s">
+        <v>21</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B324" t="s">
+        <v>703</v>
+      </c>
+      <c r="C324" t="s">
+        <v>704</v>
+      </c>
+      <c r="D324" t="s">
+        <v>11</v>
+      </c>
+      <c r="E324" t="s">
+        <v>8</v>
+      </c>
+      <c r="F324" t="s">
+        <v>21</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B325" t="s">
+        <v>705</v>
+      </c>
+      <c r="C325" t="s">
+        <v>706</v>
+      </c>
+      <c r="D325" t="s">
+        <v>18</v>
+      </c>
+      <c r="E325" t="s">
+        <v>8</v>
+      </c>
+      <c r="F325" t="s">
+        <v>51</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B326" t="s">
+        <v>707</v>
+      </c>
+      <c r="C326" t="s">
+        <v>708</v>
+      </c>
+      <c r="D326" t="s">
+        <v>15</v>
+      </c>
+      <c r="E326" t="s">
+        <v>8</v>
+      </c>
+      <c r="F326" t="s">
+        <v>51</v>
+      </c>
+      <c r="G326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B327" t="s">
+        <v>709</v>
+      </c>
+      <c r="C327" t="s">
+        <v>710</v>
+      </c>
+      <c r="D327" t="s">
+        <v>200</v>
+      </c>
+      <c r="E327" t="s">
+        <v>8</v>
+      </c>
+      <c r="F327" t="s">
+        <v>52</v>
+      </c>
+      <c r="G327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B328" t="s">
+        <v>711</v>
+      </c>
+      <c r="C328" t="s">
+        <v>712</v>
+      </c>
+      <c r="D328" t="s">
+        <v>70</v>
+      </c>
+      <c r="E328" t="s">
+        <v>8</v>
+      </c>
+      <c r="F328" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B329" t="s">
+        <v>713</v>
+      </c>
+      <c r="C329" t="s">
+        <v>714</v>
+      </c>
+      <c r="D329" t="s">
+        <v>60</v>
+      </c>
+      <c r="E329" t="s">
+        <v>8</v>
+      </c>
+      <c r="F329" t="s">
+        <v>51</v>
+      </c>
+      <c r="G329">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B330" t="s">
+        <v>715</v>
+      </c>
+      <c r="C330" t="s">
+        <v>716</v>
+      </c>
+      <c r="D330" t="s">
+        <v>200</v>
+      </c>
+      <c r="E330" t="s">
+        <v>8</v>
+      </c>
+      <c r="F330" t="s">
+        <v>21</v>
+      </c>
+      <c r="G330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B331" t="s">
+        <v>717</v>
+      </c>
+      <c r="C331" t="s">
+        <v>718</v>
+      </c>
+      <c r="D331" t="s">
+        <v>18</v>
+      </c>
+      <c r="E331" t="s">
+        <v>8</v>
+      </c>
+      <c r="F331" t="s">
+        <v>21</v>
+      </c>
+      <c r="G331">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B332" t="s">
+        <v>719</v>
+      </c>
+      <c r="C332" t="s">
+        <v>720</v>
+      </c>
+      <c r="D332" t="s">
+        <v>86</v>
+      </c>
+      <c r="E332" t="s">
+        <v>13</v>
+      </c>
+      <c r="F332" t="s">
+        <v>21</v>
+      </c>
+      <c r="G332">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B333" t="s">
+        <v>721</v>
+      </c>
+      <c r="C333" t="s">
+        <v>722</v>
+      </c>
+      <c r="D333" t="s">
+        <v>40</v>
+      </c>
+      <c r="E333" t="s">
+        <v>8</v>
+      </c>
+      <c r="F333" t="s">
+        <v>21</v>
+      </c>
+      <c r="G333">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B334" t="s">
+        <v>723</v>
+      </c>
+      <c r="C334" t="s">
+        <v>724</v>
+      </c>
+      <c r="D334" t="s">
+        <v>15</v>
+      </c>
+      <c r="E334" t="s">
+        <v>8</v>
+      </c>
+      <c r="F334" t="s">
+        <v>51</v>
+      </c>
+      <c r="G334">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>46058</v>
+      </c>
+      <c r="B335" t="s">
+        <v>725</v>
+      </c>
+      <c r="C335" t="s">
+        <v>726</v>
+      </c>
+      <c r="D335" t="s">
+        <v>262</v>
+      </c>
+      <c r="E335" t="s">
+        <v>8</v>
+      </c>
+      <c r="F335" t="s">
+        <v>51</v>
+      </c>
+      <c r="G335">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B336" t="s">
+        <v>727</v>
+      </c>
+      <c r="C336" t="s">
+        <v>728</v>
+      </c>
+      <c r="D336" t="s">
+        <v>12</v>
+      </c>
+      <c r="E336" t="s">
+        <v>8</v>
+      </c>
+      <c r="F336" t="s">
+        <v>21</v>
+      </c>
+      <c r="G336">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B337" t="s">
+        <v>729</v>
+      </c>
+      <c r="C337" t="s">
+        <v>730</v>
+      </c>
+      <c r="D337" t="s">
+        <v>40</v>
+      </c>
+      <c r="E337" t="s">
+        <v>10</v>
+      </c>
+      <c r="F337" t="s">
+        <v>21</v>
+      </c>
+      <c r="G337">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B338" t="s">
+        <v>731</v>
+      </c>
+      <c r="C338" t="s">
+        <v>732</v>
+      </c>
+      <c r="D338" t="s">
+        <v>11</v>
+      </c>
+      <c r="E338" t="s">
+        <v>8</v>
+      </c>
+      <c r="F338" t="s">
+        <v>21</v>
+      </c>
+      <c r="G338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B339" t="s">
+        <v>733</v>
+      </c>
+      <c r="C339" t="s">
+        <v>734</v>
+      </c>
+      <c r="D339" t="s">
+        <v>110</v>
+      </c>
+      <c r="E339" t="s">
+        <v>8</v>
+      </c>
+      <c r="F339" t="s">
+        <v>21</v>
+      </c>
+      <c r="G339">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B340" t="s">
+        <v>735</v>
+      </c>
+      <c r="C340" t="s">
+        <v>736</v>
+      </c>
+      <c r="D340" t="s">
+        <v>152</v>
+      </c>
+      <c r="E340" t="s">
+        <v>10</v>
+      </c>
+      <c r="F340" t="s">
+        <v>21</v>
+      </c>
+      <c r="G340">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B341" t="s">
+        <v>737</v>
+      </c>
+      <c r="C341" t="s">
+        <v>738</v>
+      </c>
+      <c r="D341" t="s">
+        <v>67</v>
+      </c>
+      <c r="E341" t="s">
+        <v>10</v>
+      </c>
+      <c r="F341" t="s">
+        <v>21</v>
+      </c>
+      <c r="G341">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>46059</v>
+      </c>
+      <c r="B342" t="s">
+        <v>739</v>
+      </c>
+      <c r="C342" t="s">
+        <v>740</v>
+      </c>
+      <c r="D342" t="s">
+        <v>9</v>
+      </c>
+      <c r="E342" t="s">
+        <v>7</v>
+      </c>
+      <c r="F342" t="s">
+        <v>21</v>
+      </c>
+      <c r="G342">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated balde and producao - base 11/02/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-02.xlsx
+++ b/first-atlas/producao_2026-02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29805"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29808"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0698F184-A08A-4D46-9509-BB95887C879E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3807D919-A0A9-47CB-A06B-2535C7BEC2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="21840" windowHeight="13290" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1227">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -3336,6 +3336,390 @@
   </si>
   <si>
     <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Certificado de Inova simples</t>
+  </si>
+  <si>
+    <t>63438186000185</t>
+  </si>
+  <si>
+    <t>J&amp;V STORE LTDA</t>
+  </si>
+  <si>
+    <t>54665244000112</t>
+  </si>
+  <si>
+    <t>TRANSPORTE CRISTINA LTDA</t>
+  </si>
+  <si>
+    <t>11233505000112</t>
+  </si>
+  <si>
+    <t>ROSY ESTEVES ENCARNACAO LTDA</t>
+  </si>
+  <si>
+    <t>22736165000169</t>
+  </si>
+  <si>
+    <t>JEAN CARLOS AVELINO PEREIRA DE BARROS</t>
+  </si>
+  <si>
+    <t>39145774000146</t>
+  </si>
+  <si>
+    <t>QUALITY CONSTRUCOES E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>14779669000138</t>
+  </si>
+  <si>
+    <t>AMAZON GEOGRAPHIC HOTEIS E TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>25333086000103</t>
+  </si>
+  <si>
+    <t>MARIA APARECIDA PADRE DA SILVA SOUSA 08611199405</t>
+  </si>
+  <si>
+    <t>14972560000112</t>
+  </si>
+  <si>
+    <t>KM JEANS CONFECCOES LTDA</t>
+  </si>
+  <si>
+    <t>33988761000152</t>
+  </si>
+  <si>
+    <t>FILIPE ROSA DA SILVA ENERGIA SOLAR</t>
+  </si>
+  <si>
+    <t>44131714000104</t>
+  </si>
+  <si>
+    <t>PARK INTERATIVO EVENTOS LTDA</t>
+  </si>
+  <si>
+    <t>64972929000165</t>
+  </si>
+  <si>
+    <t>BRASIL &amp; USA TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>50698537000145</t>
+  </si>
+  <si>
+    <t>SERVICO DE INSPECAO VEICULAR KM 32 LTDA</t>
+  </si>
+  <si>
+    <t>64854886000113</t>
+  </si>
+  <si>
+    <t>GLL SOLUCOES CONTABEIS LTDA</t>
+  </si>
+  <si>
+    <t>57801824000188</t>
+  </si>
+  <si>
+    <t>ISA RANGEL COMERCIO VAREJISTA DE ROUPAS LTDA</t>
+  </si>
+  <si>
+    <t>58419682000151</t>
+  </si>
+  <si>
+    <t>MASTER EM CONSORCIOS LTDA</t>
+  </si>
+  <si>
+    <t>64813988000190</t>
+  </si>
+  <si>
+    <t>GMDC CONSULTORIA AMBIENTAL LTDA</t>
+  </si>
+  <si>
+    <t>15815893000109</t>
+  </si>
+  <si>
+    <t>MARCENARIA AMAZONAS LIMITADA</t>
+  </si>
+  <si>
+    <t>09308808000105</t>
+  </si>
+  <si>
+    <t>DIAS E LIRA LTDA</t>
+  </si>
+  <si>
+    <t>28288285000127</t>
+  </si>
+  <si>
+    <t>CONSTRUVILLE ENGENHARIA E CONSTRUCOES LTDA</t>
+  </si>
+  <si>
+    <t>64923951000115</t>
+  </si>
+  <si>
+    <t>CARRO CERTO VEICULOS LTDA</t>
+  </si>
+  <si>
+    <t>64904270000100</t>
+  </si>
+  <si>
+    <t>DANIEL BARBOSA TERRA LTDA</t>
+  </si>
+  <si>
+    <t>Ana Carla Ferreira Fellippini</t>
+  </si>
+  <si>
+    <t>38949358000138</t>
+  </si>
+  <si>
+    <t>FORMULA USINAGEM LTDA</t>
+  </si>
+  <si>
+    <t>43689760000160</t>
+  </si>
+  <si>
+    <t>POWER TECH GMC LTDA</t>
+  </si>
+  <si>
+    <t>60748069000120</t>
+  </si>
+  <si>
+    <t>EDY FABRICACAO E MONTAGENS LTDA</t>
+  </si>
+  <si>
+    <t>58970777000169</t>
+  </si>
+  <si>
+    <t>WELISON CASTIONI FERREIRA</t>
+  </si>
+  <si>
+    <t>Ana Clara Sabio de Souza</t>
+  </si>
+  <si>
+    <t>31245109000112</t>
+  </si>
+  <si>
+    <t>TAISA MIRELA MESSIAS DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>40129863000188</t>
+  </si>
+  <si>
+    <t>GILSTON DE PAULA</t>
+  </si>
+  <si>
+    <t>64753679000172</t>
+  </si>
+  <si>
+    <t>TATIANA FREIRE SERVICOS ADMINISTRATIVOS</t>
+  </si>
+  <si>
+    <t>64863917000100</t>
+  </si>
+  <si>
+    <t>NALDO REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>Ana Laura Rodrigues da Silva</t>
+  </si>
+  <si>
+    <t>52102556000192</t>
+  </si>
+  <si>
+    <t>MONTA RJ - MONTAGENS INDUSTRIAIS LTDA</t>
+  </si>
+  <si>
+    <t>64980093000140</t>
+  </si>
+  <si>
+    <t>BOM - SERVICOS MEDICOS DE APOIO A SAUDE LTDA</t>
+  </si>
+  <si>
+    <t>47142388000129</t>
+  </si>
+  <si>
+    <t>MIRIAN BARBOSA DA SILVA</t>
+  </si>
+  <si>
+    <t>08491873000156</t>
+  </si>
+  <si>
+    <t>TAKAMORI GESTAO EMPRESARIAL LTDA</t>
+  </si>
+  <si>
+    <t>49629584000158</t>
+  </si>
+  <si>
+    <t>MAAF CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>39604808000113</t>
+  </si>
+  <si>
+    <t>PRESENZA CAR AUTO CENTER LTDA</t>
+  </si>
+  <si>
+    <t>46545911000103</t>
+  </si>
+  <si>
+    <t>POUSADA BRASIL TURISMO LTDA</t>
+  </si>
+  <si>
+    <t>26337655000143</t>
+  </si>
+  <si>
+    <t>JOSE ALFREDO MUSSI DE SOUZA &amp; CIA LTDA</t>
+  </si>
+  <si>
+    <t>TPG</t>
+  </si>
+  <si>
+    <t>18222665000105</t>
+  </si>
+  <si>
+    <t>MADEREIRA ALIANCA LTDA</t>
+  </si>
+  <si>
+    <t>13461347000183</t>
+  </si>
+  <si>
+    <t>LUAU PRODUCOES E EVENTOS LIMITADA</t>
+  </si>
+  <si>
+    <t>57505002000150</t>
+  </si>
+  <si>
+    <t>57.505.002 JOSELI VIEIRA DOS SANTOS SILVA</t>
+  </si>
+  <si>
+    <t>65000115000121</t>
+  </si>
+  <si>
+    <t>B&amp;R IMOBILIARIOS LTDA</t>
+  </si>
+  <si>
+    <t>40095178000188</t>
+  </si>
+  <si>
+    <t>BARBER HAUSS BARBEARIA LTDA</t>
+  </si>
+  <si>
+    <t>64289840000107</t>
+  </si>
+  <si>
+    <t>NP REPRESENTACOES COMERCIAL LTDA</t>
+  </si>
+  <si>
+    <t>52889231000100</t>
+  </si>
+  <si>
+    <t>SS ROCHA ASSESSORIA E CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>64986006000162</t>
+  </si>
+  <si>
+    <t>POUSADA E KIOSQUE DAG E JULIO LTDA</t>
+  </si>
+  <si>
+    <t>60813940000121</t>
+  </si>
+  <si>
+    <t>ITAVERAVA TRANSPORTES</t>
+  </si>
+  <si>
+    <t>41414527000140</t>
+  </si>
+  <si>
+    <t>VANESSA BARBOSA CHIOVETTI MORAES CONSULTORIO ODONTOLOGICO LTDA</t>
+  </si>
+  <si>
+    <t>39964872000105</t>
+  </si>
+  <si>
+    <t>39.964.872 NATALIA FAUSTO DINIZ MARTINS</t>
+  </si>
+  <si>
+    <t>62360809000181</t>
+  </si>
+  <si>
+    <t>INSTITUTO TEMPO DE CUIDAR CARETIME LTDA</t>
+  </si>
+  <si>
+    <t>62411121000183</t>
+  </si>
+  <si>
+    <t>K&amp;G AUTOMACAO INDUSTRIAL LTDA</t>
+  </si>
+  <si>
+    <t>64805962000109</t>
+  </si>
+  <si>
+    <t>MV VIDROS LTDA</t>
+  </si>
+  <si>
+    <t>11812991000123</t>
+  </si>
+  <si>
+    <t>MAQJOB LOCACAO DE MAQUINAS LTDA</t>
+  </si>
+  <si>
+    <t>60612366000143</t>
+  </si>
+  <si>
+    <t>EMINENTES FORMATURAS LTDA</t>
+  </si>
+  <si>
+    <t>34667260000137</t>
+  </si>
+  <si>
+    <t>LOPES BAR E LANCHONETE LTDA</t>
+  </si>
+  <si>
+    <t>20667781000180</t>
+  </si>
+  <si>
+    <t>ANDREIA MARIA PIMENTEL</t>
+  </si>
+  <si>
+    <t>37129220000120</t>
+  </si>
+  <si>
+    <t>O S J CONSTRUCOES LTDA</t>
+  </si>
+  <si>
+    <t>64990822000140</t>
+  </si>
+  <si>
+    <t>JARDEL SANTANA LTDA</t>
+  </si>
+  <si>
+    <t>15811504000169</t>
+  </si>
+  <si>
+    <t>TATIANE KELEN TEBAR</t>
+  </si>
+  <si>
+    <t>44961087000139</t>
+  </si>
+  <si>
+    <t>GRUPO NOVA ERA COMERCIO DE AUTOMOVEIS LTDA</t>
+  </si>
+  <si>
+    <t>63835109000169</t>
+  </si>
+  <si>
+    <t>E M T COMERCIO DE MAQUINAS E SERVICE AMBIENTAIS LTDA</t>
+  </si>
+  <si>
+    <t>35196665000105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIAGO JUNIO ALVES DA SILVA </t>
+  </si>
+  <si>
+    <t>50217786000171</t>
+  </si>
+  <si>
+    <t>PRIME SERVICE ASSEIO E CONSERVACAO LTDA</t>
   </si>
 </sst>
 </file>
@@ -3708,10 +4092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A45A88-3D17-4433-986A-11075963C36F}">
-  <dimension ref="A1:G519"/>
+  <dimension ref="A1:G581"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,7 +4534,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -5481,7 +5865,7 @@
         <v>10</v>
       </c>
       <c r="F77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -6746,7 +7130,7 @@
         <v>8</v>
       </c>
       <c r="F132" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="G132" t="s">
         <v>440</v>
@@ -7390,7 +7774,7 @@
         <v>8</v>
       </c>
       <c r="F160" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G160">
         <v>0</v>
@@ -9253,10 +9637,10 @@
         <v>8</v>
       </c>
       <c r="F241" t="s">
-        <v>50</v>
-      </c>
-      <c r="G241" t="s">
-        <v>262</v>
+        <v>21</v>
+      </c>
+      <c r="G241">
+        <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -11185,7 +11569,7 @@
         <v>8</v>
       </c>
       <c r="F325" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="G325">
         <v>0</v>
@@ -13846,6 +14230,9 @@
       <c r="F441" t="s">
         <v>21</v>
       </c>
+      <c r="G441">
+        <v>0</v>
+      </c>
     </row>
     <row r="442" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
@@ -14117,7 +14504,7 @@
         <v>8</v>
       </c>
       <c r="F453" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G453">
         <v>0</v>
@@ -14163,7 +14550,7 @@
         <v>8</v>
       </c>
       <c r="F455" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G455">
         <v>0</v>
@@ -14186,7 +14573,7 @@
         <v>7</v>
       </c>
       <c r="F456" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G456">
         <v>0</v>
@@ -14209,7 +14596,7 @@
         <v>8</v>
       </c>
       <c r="F457" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G457">
         <v>0</v>
@@ -14485,7 +14872,7 @@
         <v>8</v>
       </c>
       <c r="F469" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G469">
         <v>0</v>
@@ -14508,7 +14895,7 @@
         <v>8</v>
       </c>
       <c r="F470" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G470">
         <v>0</v>
@@ -14554,7 +14941,7 @@
         <v>7</v>
       </c>
       <c r="F472" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G472">
         <v>0</v>
@@ -14577,7 +14964,7 @@
         <v>8</v>
       </c>
       <c r="F473" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G473">
         <v>0</v>
@@ -14600,7 +14987,7 @@
         <v>10</v>
       </c>
       <c r="F474" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G474">
         <v>0</v>
@@ -14853,7 +15240,7 @@
         <v>8</v>
       </c>
       <c r="F485" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G485">
         <v>0</v>
@@ -14945,7 +15332,7 @@
         <v>7</v>
       </c>
       <c r="F489" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G489">
         <v>0</v>
@@ -15037,7 +15424,7 @@
         <v>118</v>
       </c>
       <c r="F493" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="G493">
         <v>0</v>
@@ -15175,7 +15562,7 @@
         <v>10</v>
       </c>
       <c r="F499" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G499">
         <v>0</v>
@@ -15244,7 +15631,7 @@
         <v>8</v>
       </c>
       <c r="F502" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G502">
         <v>0</v>
@@ -15405,7 +15792,7 @@
         <v>8</v>
       </c>
       <c r="F509" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G509">
         <v>0</v>
@@ -15451,7 +15838,7 @@
         <v>7</v>
       </c>
       <c r="F511" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G511">
         <v>0</v>
@@ -15497,7 +15884,7 @@
         <v>8</v>
       </c>
       <c r="F513" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G513">
         <v>0</v>
@@ -15520,7 +15907,7 @@
         <v>8</v>
       </c>
       <c r="F514" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G514">
         <v>0</v>
@@ -15582,6 +15969,12 @@
       <c r="C517" t="s">
         <v>1091</v>
       </c>
+      <c r="D517" t="s">
+        <v>59</v>
+      </c>
+      <c r="E517" t="s">
+        <v>8</v>
+      </c>
       <c r="F517" t="s">
         <v>21</v>
       </c>
@@ -15632,6 +16025,1429 @@
         <v>21</v>
       </c>
       <c r="G519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A520" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B520" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C520" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D520" t="s">
+        <v>24</v>
+      </c>
+      <c r="E520" t="s">
+        <v>8</v>
+      </c>
+      <c r="F520" t="s">
+        <v>21</v>
+      </c>
+      <c r="G520">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A521" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B521" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C521" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D521" t="s">
+        <v>18</v>
+      </c>
+      <c r="E521" t="s">
+        <v>8</v>
+      </c>
+      <c r="F521" t="s">
+        <v>50</v>
+      </c>
+      <c r="G521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A522" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B522" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C522" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D522" t="s">
+        <v>210</v>
+      </c>
+      <c r="E522" t="s">
+        <v>7</v>
+      </c>
+      <c r="F522" t="s">
+        <v>21</v>
+      </c>
+      <c r="G522">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A523" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B523" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C523" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D523" t="s">
+        <v>261</v>
+      </c>
+      <c r="E523" t="s">
+        <v>8</v>
+      </c>
+      <c r="F523" t="s">
+        <v>50</v>
+      </c>
+      <c r="G523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A524" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B524" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C524" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D524" t="s">
+        <v>19</v>
+      </c>
+      <c r="E524" t="s">
+        <v>8</v>
+      </c>
+      <c r="F524" t="s">
+        <v>50</v>
+      </c>
+      <c r="G524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A525" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B525" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C525" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D525" t="s">
+        <v>9</v>
+      </c>
+      <c r="E525" t="s">
+        <v>7</v>
+      </c>
+      <c r="F525" t="s">
+        <v>50</v>
+      </c>
+      <c r="G525">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A526" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B526" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C526" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D526" t="s">
+        <v>17</v>
+      </c>
+      <c r="E526" t="s">
+        <v>7</v>
+      </c>
+      <c r="F526" t="s">
+        <v>21</v>
+      </c>
+      <c r="G526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A527" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B527" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C527" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D527" t="s">
+        <v>12</v>
+      </c>
+      <c r="E527" t="s">
+        <v>7</v>
+      </c>
+      <c r="F527" t="s">
+        <v>50</v>
+      </c>
+      <c r="G527">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A528" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B528" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C528" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D528" t="s">
+        <v>896</v>
+      </c>
+      <c r="E528" t="s">
+        <v>7</v>
+      </c>
+      <c r="F528" t="s">
+        <v>21</v>
+      </c>
+      <c r="G528">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A529" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B529" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C529" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D529" t="s">
+        <v>85</v>
+      </c>
+      <c r="E529" t="s">
+        <v>7</v>
+      </c>
+      <c r="F529" t="s">
+        <v>21</v>
+      </c>
+      <c r="G529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A530" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C530" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D530" t="s">
+        <v>162</v>
+      </c>
+      <c r="E530" t="s">
+        <v>10</v>
+      </c>
+      <c r="F530" t="s">
+        <v>21</v>
+      </c>
+      <c r="G530">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A531" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C531" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D531" t="s">
+        <v>12</v>
+      </c>
+      <c r="E531" t="s">
+        <v>7</v>
+      </c>
+      <c r="F531" t="s">
+        <v>50</v>
+      </c>
+      <c r="G531">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A532" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C532" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D532" t="s">
+        <v>19</v>
+      </c>
+      <c r="E532" t="s">
+        <v>7</v>
+      </c>
+      <c r="F532" t="s">
+        <v>50</v>
+      </c>
+      <c r="G532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A533" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B533" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C533" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D533" t="s">
+        <v>16</v>
+      </c>
+      <c r="E533" t="s">
+        <v>8</v>
+      </c>
+      <c r="F533" t="s">
+        <v>112</v>
+      </c>
+      <c r="G533" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A534" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B534" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C534" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D534" t="s">
+        <v>15</v>
+      </c>
+      <c r="E534" t="s">
+        <v>8</v>
+      </c>
+      <c r="F534" t="s">
+        <v>21</v>
+      </c>
+      <c r="G534">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A535" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B535" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C535" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D535" t="s">
+        <v>75</v>
+      </c>
+      <c r="E535" t="s">
+        <v>10</v>
+      </c>
+      <c r="F535" t="s">
+        <v>50</v>
+      </c>
+      <c r="G535">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A536" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B536" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C536" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D536" t="s">
+        <v>16</v>
+      </c>
+      <c r="E536" t="s">
+        <v>8</v>
+      </c>
+      <c r="F536" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A537" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B537" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C537" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D537" t="s">
+        <v>261</v>
+      </c>
+      <c r="E537" t="s">
+        <v>8</v>
+      </c>
+      <c r="F537" t="s">
+        <v>21</v>
+      </c>
+      <c r="G537">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A538" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B538" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C538" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D538" t="s">
+        <v>11</v>
+      </c>
+      <c r="E538" t="s">
+        <v>8</v>
+      </c>
+      <c r="F538" t="s">
+        <v>51</v>
+      </c>
+      <c r="G538">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A539" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B539" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C539" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D539" t="s">
+        <v>66</v>
+      </c>
+      <c r="E539" t="s">
+        <v>190</v>
+      </c>
+      <c r="F539" t="s">
+        <v>21</v>
+      </c>
+      <c r="G539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A540" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B540" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C540" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D540" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E540" t="s">
+        <v>10</v>
+      </c>
+      <c r="F540" t="s">
+        <v>21</v>
+      </c>
+      <c r="G540">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A541" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B541" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C541" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D541" t="s">
+        <v>11</v>
+      </c>
+      <c r="E541" t="s">
+        <v>8</v>
+      </c>
+      <c r="F541" t="s">
+        <v>50</v>
+      </c>
+      <c r="G541">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A542" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B542" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C542" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D542" t="s">
+        <v>59</v>
+      </c>
+      <c r="E542" t="s">
+        <v>8</v>
+      </c>
+      <c r="F542" t="s">
+        <v>50</v>
+      </c>
+      <c r="G542">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A543" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B543" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C543" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D543" t="s">
+        <v>11</v>
+      </c>
+      <c r="E543" t="s">
+        <v>8</v>
+      </c>
+      <c r="F543" t="s">
+        <v>21</v>
+      </c>
+      <c r="G543">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A544" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B544" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C544" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D544" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E544" t="s">
+        <v>7</v>
+      </c>
+      <c r="F544" t="s">
+        <v>21</v>
+      </c>
+      <c r="G544">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A545" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B545" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C545" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D545" t="s">
+        <v>261</v>
+      </c>
+      <c r="E545" t="s">
+        <v>8</v>
+      </c>
+      <c r="F545" t="s">
+        <v>51</v>
+      </c>
+      <c r="G545">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A546" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B546" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C546" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D546" t="s">
+        <v>16</v>
+      </c>
+      <c r="E546" t="s">
+        <v>8</v>
+      </c>
+      <c r="F546" t="s">
+        <v>21</v>
+      </c>
+      <c r="G546">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A547" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B547" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C547" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D547" t="s">
+        <v>18</v>
+      </c>
+      <c r="E547" t="s">
+        <v>8</v>
+      </c>
+      <c r="F547" t="s">
+        <v>21</v>
+      </c>
+      <c r="G547">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A548" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B548" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C548" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D548" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E548" t="s">
+        <v>10</v>
+      </c>
+      <c r="F548" t="s">
+        <v>21</v>
+      </c>
+      <c r="G548">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A549" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B549" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C549" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D549" t="s">
+        <v>9</v>
+      </c>
+      <c r="E549" t="s">
+        <v>8</v>
+      </c>
+      <c r="F549" t="s">
+        <v>50</v>
+      </c>
+      <c r="G549">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A550" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B550" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C550" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D550" t="s">
+        <v>75</v>
+      </c>
+      <c r="E550" t="s">
+        <v>10</v>
+      </c>
+      <c r="F550" t="s">
+        <v>50</v>
+      </c>
+      <c r="G550">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A551" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B551" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C551" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D551" t="s">
+        <v>9</v>
+      </c>
+      <c r="E551" t="s">
+        <v>8</v>
+      </c>
+      <c r="F551" t="s">
+        <v>21</v>
+      </c>
+      <c r="G551">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A552" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B552" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C552" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D552" t="s">
+        <v>19</v>
+      </c>
+      <c r="E552" t="s">
+        <v>7</v>
+      </c>
+      <c r="F552" t="s">
+        <v>21</v>
+      </c>
+      <c r="G552">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A553" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B553" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C553" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D553" t="s">
+        <v>162</v>
+      </c>
+      <c r="E553" t="s">
+        <v>8</v>
+      </c>
+      <c r="F553" t="s">
+        <v>21</v>
+      </c>
+      <c r="G553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A554" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B554" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C554" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D554" t="s">
+        <v>72</v>
+      </c>
+      <c r="E554" t="s">
+        <v>8</v>
+      </c>
+      <c r="F554" t="s">
+        <v>21</v>
+      </c>
+      <c r="G554">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A555" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B555" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C555" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D555" t="s">
+        <v>15</v>
+      </c>
+      <c r="E555" t="s">
+        <v>8</v>
+      </c>
+      <c r="F555" t="s">
+        <v>21</v>
+      </c>
+      <c r="G555">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A556" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B556" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C556" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D556" t="s">
+        <v>261</v>
+      </c>
+      <c r="E556" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F556" t="s">
+        <v>51</v>
+      </c>
+      <c r="G556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A557" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B557" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C557" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D557" t="s">
+        <v>11</v>
+      </c>
+      <c r="E557" t="s">
+        <v>8</v>
+      </c>
+      <c r="F557" t="s">
+        <v>21</v>
+      </c>
+      <c r="G557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A558" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B558" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C558" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D558" t="s">
+        <v>210</v>
+      </c>
+      <c r="E558" t="s">
+        <v>7</v>
+      </c>
+      <c r="F558" t="s">
+        <v>50</v>
+      </c>
+      <c r="G558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A559" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B559" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C559" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D559" t="s">
+        <v>261</v>
+      </c>
+      <c r="E559" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F559" t="s">
+        <v>21</v>
+      </c>
+      <c r="G559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A560" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B560" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C560" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D560" t="s">
+        <v>75</v>
+      </c>
+      <c r="E560" t="s">
+        <v>10</v>
+      </c>
+      <c r="F560" t="s">
+        <v>50</v>
+      </c>
+      <c r="G560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A561" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B561" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C561" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D561" t="s">
+        <v>151</v>
+      </c>
+      <c r="E561" t="s">
+        <v>8</v>
+      </c>
+      <c r="F561" t="s">
+        <v>21</v>
+      </c>
+      <c r="G561">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A562" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C562" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D562" t="s">
+        <v>39</v>
+      </c>
+      <c r="E562" t="s">
+        <v>8</v>
+      </c>
+      <c r="F562" t="s">
+        <v>21</v>
+      </c>
+      <c r="G562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A563" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B563" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C563" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D563" t="s">
+        <v>199</v>
+      </c>
+      <c r="E563" t="s">
+        <v>8</v>
+      </c>
+      <c r="F563" t="s">
+        <v>21</v>
+      </c>
+      <c r="G563">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A564" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B564" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C564" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D564" t="s">
+        <v>162</v>
+      </c>
+      <c r="E564" t="s">
+        <v>10</v>
+      </c>
+      <c r="F564" t="s">
+        <v>50</v>
+      </c>
+      <c r="G564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A565" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B565" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C565" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D565" t="s">
+        <v>39</v>
+      </c>
+      <c r="E565" t="s">
+        <v>8</v>
+      </c>
+      <c r="F565" t="s">
+        <v>21</v>
+      </c>
+      <c r="G565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A566" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B566" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C566" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D566" t="s">
+        <v>18</v>
+      </c>
+      <c r="E566" t="s">
+        <v>8</v>
+      </c>
+      <c r="F566" t="s">
+        <v>112</v>
+      </c>
+      <c r="G566">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A567" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B567" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C567" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D567" t="s">
+        <v>261</v>
+      </c>
+      <c r="E567" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F567" t="s">
+        <v>21</v>
+      </c>
+      <c r="G567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A568" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B568" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C568" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D568" t="s">
+        <v>59</v>
+      </c>
+      <c r="E568" t="s">
+        <v>8</v>
+      </c>
+      <c r="F568" t="s">
+        <v>21</v>
+      </c>
+      <c r="G568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A569" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B569" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C569" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D569" t="s">
+        <v>72</v>
+      </c>
+      <c r="E569" t="s">
+        <v>8</v>
+      </c>
+      <c r="F569" t="s">
+        <v>51</v>
+      </c>
+      <c r="G569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A570" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B570" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C570" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D570" t="s">
+        <v>75</v>
+      </c>
+      <c r="E570" t="s">
+        <v>10</v>
+      </c>
+      <c r="F570" t="s">
+        <v>51</v>
+      </c>
+      <c r="G570">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A571" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B571" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C571" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D571" t="s">
+        <v>12</v>
+      </c>
+      <c r="E571" t="s">
+        <v>8</v>
+      </c>
+      <c r="F571" t="s">
+        <v>112</v>
+      </c>
+      <c r="G571" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A572" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B572" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C572" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D572" t="s">
+        <v>18</v>
+      </c>
+      <c r="E572" t="s">
+        <v>8</v>
+      </c>
+      <c r="F572" t="s">
+        <v>51</v>
+      </c>
+      <c r="G572">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A573" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B573" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C573" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D573" t="s">
+        <v>59</v>
+      </c>
+      <c r="E573" t="s">
+        <v>8</v>
+      </c>
+      <c r="F573" t="s">
+        <v>21</v>
+      </c>
+      <c r="G573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A574" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B574" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C574" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D574" t="s">
+        <v>16</v>
+      </c>
+      <c r="E574" t="s">
+        <v>8</v>
+      </c>
+      <c r="F574" t="s">
+        <v>21</v>
+      </c>
+      <c r="G574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A575" s="1">
+        <v>46063</v>
+      </c>
+      <c r="B575" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C575" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D575" t="s">
+        <v>18</v>
+      </c>
+      <c r="E575" t="s">
+        <v>7</v>
+      </c>
+      <c r="F575" t="s">
+        <v>50</v>
+      </c>
+      <c r="G575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A576" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B576" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C576" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D576" t="s">
+        <v>151</v>
+      </c>
+      <c r="E576" t="s">
+        <v>10</v>
+      </c>
+      <c r="F576" t="s">
+        <v>21</v>
+      </c>
+      <c r="G576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A577" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B577" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C577" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D577" t="s">
+        <v>261</v>
+      </c>
+      <c r="E577" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F577" t="s">
+        <v>21</v>
+      </c>
+      <c r="G577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A578" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C578" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D578" t="s">
+        <v>12</v>
+      </c>
+      <c r="E578" t="s">
+        <v>8</v>
+      </c>
+      <c r="F578" t="s">
+        <v>21</v>
+      </c>
+      <c r="G578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A579" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B579" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C579" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D579" t="s">
+        <v>78</v>
+      </c>
+      <c r="E579" t="s">
+        <v>10</v>
+      </c>
+      <c r="F579" t="s">
+        <v>21</v>
+      </c>
+      <c r="G579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A580" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C580" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D580" t="s">
+        <v>12</v>
+      </c>
+      <c r="E580" t="s">
+        <v>8</v>
+      </c>
+      <c r="F580" t="s">
+        <v>21</v>
+      </c>
+      <c r="G580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A581" s="1">
+        <v>46064</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C581" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D581" t="s">
+        <v>199</v>
+      </c>
+      <c r="E581" t="s">
+        <v>8</v>
+      </c>
+      <c r="F581" t="s">
+        <v>21</v>
+      </c>
+      <c r="G581">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated balde - base 24/02/2026
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2026-02.xlsx
+++ b/first-atlas/producao_2026-02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6396F550-E86D-42B9-A2D9-7406C351D97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F682F3E5-1B48-42C3-A026-254E48016FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F5572131-3C84-4D9C-B555-72DCC3B1940B}"/>
   </bookViews>
@@ -7776,7 +7776,7 @@
   <dimension ref="A1:G1186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>